<commit_message>
Fully working prototype V1
</commit_message>
<xml_diff>
--- a/data/poc_details.xlsx
+++ b/data/poc_details.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faisa\OneDrive\Desktop\secure-email-sender\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faisa\OneDrive\Desktop\email-sender\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F32263A-19C9-4E1B-875A-727E613B25CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880CD64D-2406-4940-8899-C8C9123F9ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="1515" windowWidth="21600" windowHeight="11295" xr2:uid="{771CDB77-B6A1-46EA-A912-05EC9CE7ACE9}"/>
+    <workbookView xWindow="3765" yWindow="3675" windowWidth="21600" windowHeight="11295" xr2:uid="{771CDB77-B6A1-46EA-A912-05EC9CE7ACE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,63 +36,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>poc_name</t>
-  </si>
-  <si>
-    <t>poc_designation</t>
-  </si>
-  <si>
-    <t>poc_contact</t>
-  </si>
-  <si>
-    <t>poc_email</t>
-  </si>
-  <si>
-    <t>department</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Faisal</t>
   </si>
   <si>
-    <t>Coordinator</t>
-  </si>
-  <si>
-    <t>faisalmuhiuddin@gmail.com</t>
-  </si>
-  <si>
-    <t>Biotech</t>
-  </si>
-  <si>
-    <t>AAS</t>
-  </si>
-  <si>
-    <t>Secretary</t>
-  </si>
-  <si>
-    <t>sec_acaf@smail.iitm.ac.in</t>
-  </si>
-  <si>
-    <t>Chemical</t>
+    <t>POC_name</t>
+  </si>
+  <si>
+    <t>POC_designation</t>
+  </si>
+  <si>
+    <t>POC_contact</t>
+  </si>
+  <si>
+    <t>Aryan</t>
+  </si>
+  <si>
+    <t>Deputy Coordinator</t>
+  </si>
+  <si>
+    <t>Aditya</t>
+  </si>
+  <si>
+    <t>Head</t>
+  </si>
+  <si>
+    <t>Placement Coordinator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,16 +95,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -457,77 +434,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35929D04-74F0-4CB3-A6E2-FBBE7675CC8C}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>8960660510</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>8420933451</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
+      <c r="C4">
+        <v>1000000000</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{96C3B8BC-8392-4C99-94E0-0985632C3879}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{A5248D9C-2762-4BF6-8B81-0C575B48803C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added heads in POC
</commit_message>
<xml_diff>
--- a/data/poc_details.xlsx
+++ b/data/poc_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faisa\OneDrive\Desktop\email-sender\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880CD64D-2406-4940-8899-C8C9123F9ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF2C241-F20E-452B-831F-D2A849C2BD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="3675" windowWidth="21600" windowHeight="11295" xr2:uid="{771CDB77-B6A1-46EA-A912-05EC9CE7ACE9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{771CDB77-B6A1-46EA-A912-05EC9CE7ACE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Faisal</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>POC_name</t>
   </si>
@@ -50,19 +47,19 @@
     <t>POC_contact</t>
   </si>
   <si>
-    <t>Aryan</t>
-  </si>
-  <si>
-    <t>Deputy Coordinator</t>
-  </si>
-  <si>
-    <t>Aditya</t>
-  </si>
-  <si>
     <t>Head</t>
   </si>
   <si>
     <t>Placement Coordinator</t>
+  </si>
+  <si>
+    <t>Faisal Muhiuddin</t>
+  </si>
+  <si>
+    <t>Aditya Raj</t>
+  </si>
+  <si>
+    <t>Charchit Chopra</t>
   </si>
 </sst>
 </file>
@@ -442,28 +439,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>8960660510</v>
@@ -471,24 +468,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>1000000000</v>
+        <v>8160079524</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>1000000000</v>
+        <v>9893364488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>